<commit_message>
More refactoring on product stuff
</commit_message>
<xml_diff>
--- a/1_Orga/A4D_Phase1_1_Project_Plan.xlsx
+++ b/1_Orga/A4D_Phase1_1_Project_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Correlaid\A4D\a4d_analytics\1_Orga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{450391EF-564A-4D9A-9615-BF6911E1A1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA063E54-1ED7-4F68-B72E-AFFB3B48FFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5426FD3C-714E-4CD6-8EF1-D51510F1D5BC}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,8 +584,8 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -606,12 +606,12 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -633,10 +633,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="1"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="3"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>

</xml_diff>

<commit_message>
Updated project plan and todos
</commit_message>
<xml_diff>
--- a/1_Orga/A4D_Phase1_1_Project_Plan.xlsx
+++ b/1_Orga/A4D_Phase1_1_Project_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Correlaid\A4D\a4d_analytics\1_Orga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA063E54-1ED7-4F68-B72E-AFFB3B48FFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E8118C-C288-406D-BC0C-9CBF9073A3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5426FD3C-714E-4CD6-8EF1-D51510F1D5BC}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -606,8 +606,8 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>

</xml_diff>